<commit_message>
55	Rename is_success to is_path_found.
</commit_message>
<xml_diff>
--- a/benchmark/runtime.xlsx
+++ b/benchmark/runtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitcloud\libMultiRobotPlanning\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA5F34A-B1A5-4EF4-8846-BF8C9E4C0206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616FE3FF-2341-4DB4-AB9C-E819D9465C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="3007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="3008">
   <si>
     <t>map_8by8_obst12_agents10_ex0.yaml</t>
   </si>
@@ -9048,6 +9048,10 @@
   </si>
   <si>
     <t>gloriyo-mine</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5h算不出来程序被kill了</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -9460,7 +9464,7 @@
   <dimension ref="A1:E2002"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1894" workbookViewId="0">
-      <selection activeCell="C1908" sqref="C1908"/>
+      <selection activeCell="E1910" sqref="E1910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -19137,10 +19141,22 @@
       <c r="A1908" t="s">
         <v>1905</v>
       </c>
+      <c r="C1908" t="s">
+        <v>3007</v>
+      </c>
+      <c r="E1908">
+        <v>0.28599000000000002</v>
+      </c>
     </row>
     <row r="1909" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1909" t="s">
         <v>1906</v>
+      </c>
+      <c r="C1909">
+        <v>57.531999999999996</v>
+      </c>
+      <c r="E1909">
+        <v>39.853900000000003</v>
       </c>
     </row>
     <row r="1910" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
85	Move in cost add back.
</commit_message>
<xml_diff>
--- a/benchmark/runtime.xlsx
+++ b/benchmark/runtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitcloud\libMultiRobotPlanning\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616FE3FF-2341-4DB4-AB9C-E819D9465C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F7D67E-332C-4A31-9BA2-BA1F97BBA8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3011" uniqueCount="3008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="3010">
   <si>
     <t>map_8by8_obst12_agents10_ex0.yaml</t>
   </si>
@@ -9052,6 +9052,14 @@
   </si>
   <si>
     <t>1.5h算不出来程序被kill了</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gloriyo-mine-set_context</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>cost</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -9059,7 +9067,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -9077,6 +9085,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -9118,9 +9134,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -9461,109 +9480,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2002"/>
+  <dimension ref="A1:G2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1894" workbookViewId="0">
-      <selection activeCell="E1910" sqref="E1910"/>
+    <sheetView tabSelected="1" topLeftCell="A1791" workbookViewId="0">
+      <selection activeCell="B1804" sqref="B1804"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2000</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>3009</v>
+      </c>
+      <c r="C1" t="s">
         <v>2001</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2003</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2004</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3006</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>3008</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -17488,171 +17515,171 @@
         <v>1598</v>
       </c>
     </row>
-    <row r="1601" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1601" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1601" t="s">
         <v>1599</v>
       </c>
     </row>
-    <row r="1602" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1602" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1602" t="s">
         <v>1600</v>
       </c>
     </row>
-    <row r="1603" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1603" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1603" t="s">
         <v>1601</v>
       </c>
     </row>
-    <row r="1604" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1604" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1604" t="s">
         <v>1602</v>
       </c>
-      <c r="B1604">
+      <c r="C1604">
         <v>0.198824</v>
       </c>
     </row>
-    <row r="1605" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1605" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1605" t="s">
         <v>1603</v>
       </c>
     </row>
-    <row r="1606" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1606" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1606" t="s">
         <v>1604</v>
       </c>
     </row>
-    <row r="1607" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1607" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1607" t="s">
         <v>1605</v>
       </c>
     </row>
-    <row r="1608" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1608" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1608" t="s">
         <v>1606</v>
       </c>
     </row>
-    <row r="1609" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1609" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1609" t="s">
         <v>1607</v>
       </c>
     </row>
-    <row r="1610" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1610" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1610" t="s">
         <v>1608</v>
       </c>
     </row>
-    <row r="1611" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1611" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1611" t="s">
         <v>1609</v>
       </c>
     </row>
-    <row r="1612" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1612" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1612" t="s">
         <v>1610</v>
       </c>
     </row>
-    <row r="1613" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1613" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1613" t="s">
         <v>1611</v>
       </c>
     </row>
-    <row r="1614" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1614" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1614" t="s">
         <v>1612</v>
       </c>
     </row>
-    <row r="1615" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1615" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1615" t="s">
         <v>1613</v>
       </c>
-      <c r="B1615">
+      <c r="C1615">
         <v>3.9553899999999996E-3</v>
       </c>
     </row>
-    <row r="1616" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1616" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1616" t="s">
         <v>1614</v>
       </c>
     </row>
-    <row r="1617" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1617" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1617" t="s">
         <v>1615</v>
       </c>
     </row>
-    <row r="1618" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1618" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1618" t="s">
         <v>1616</v>
       </c>
     </row>
-    <row r="1619" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1619" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1619" t="s">
         <v>1617</v>
       </c>
     </row>
-    <row r="1620" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1620" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1620" t="s">
         <v>1618</v>
       </c>
     </row>
-    <row r="1621" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1621" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1621" t="s">
         <v>1619</v>
       </c>
     </row>
-    <row r="1622" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1622" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1622" t="s">
         <v>1620</v>
       </c>
     </row>
-    <row r="1623" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1623" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1623" t="s">
         <v>1621</v>
       </c>
     </row>
-    <row r="1624" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1624" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1624" t="s">
         <v>1622</v>
       </c>
     </row>
-    <row r="1625" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1625" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1625" t="s">
         <v>1623</v>
       </c>
     </row>
-    <row r="1626" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1626" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1626" t="s">
         <v>1624</v>
       </c>
-      <c r="B1626">
+      <c r="C1626">
         <v>4.3862299999999996E-3</v>
       </c>
     </row>
-    <row r="1627" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1627" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1627" t="s">
         <v>1625</v>
       </c>
     </row>
-    <row r="1628" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1628" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1628" t="s">
         <v>1626</v>
       </c>
     </row>
-    <row r="1629" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1629" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1629" t="s">
         <v>1627</v>
       </c>
     </row>
-    <row r="1630" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1630" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1630" t="s">
         <v>1628</v>
       </c>
     </row>
-    <row r="1631" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1631" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1631" t="s">
         <v>1629</v>
       </c>
     </row>
-    <row r="1632" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1632" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1632" t="s">
         <v>1630</v>
       </c>
@@ -17977,85 +18004,85 @@
         <v>1694</v>
       </c>
     </row>
-    <row r="1697" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1697" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1697" t="s">
         <v>1695</v>
       </c>
     </row>
-    <row r="1698" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1698" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1698" t="s">
         <v>1696</v>
       </c>
     </row>
-    <row r="1699" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1699" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1699" t="s">
         <v>1697</v>
       </c>
     </row>
-    <row r="1700" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1700" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1700" t="s">
         <v>1698</v>
       </c>
     </row>
-    <row r="1701" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1701" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1701" t="s">
         <v>1699</v>
       </c>
     </row>
-    <row r="1702" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1702" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1702" t="s">
         <v>1700</v>
       </c>
     </row>
-    <row r="1703" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1703" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1703" t="s">
         <v>1701</v>
       </c>
-      <c r="B1703">
+      <c r="C1703">
         <v>2.9130900000000001E-2</v>
       </c>
     </row>
-    <row r="1704" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1704" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1704" t="s">
         <v>1702</v>
       </c>
     </row>
-    <row r="1705" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1705" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1705" t="s">
         <v>1703</v>
       </c>
     </row>
-    <row r="1706" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1706" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1706" t="s">
         <v>1704</v>
       </c>
     </row>
-    <row r="1707" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1707" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1707" t="s">
         <v>1705</v>
       </c>
     </row>
-    <row r="1708" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1708" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1708" t="s">
         <v>1706</v>
       </c>
     </row>
-    <row r="1709" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1709" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1709" t="s">
         <v>1707</v>
       </c>
     </row>
-    <row r="1710" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1710" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1710" t="s">
         <v>1708</v>
       </c>
     </row>
-    <row r="1711" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1711" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1711" t="s">
         <v>1709</v>
       </c>
     </row>
-    <row r="1712" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1712" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1712" t="s">
         <v>1710</v>
       </c>
@@ -18460,240 +18487,273 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="1793" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1793" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1793" t="s">
         <v>1791</v>
       </c>
     </row>
-    <row r="1794" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1794" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1794" t="s">
         <v>1792</v>
       </c>
     </row>
-    <row r="1795" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1795" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1795" t="s">
         <v>1793</v>
       </c>
     </row>
-    <row r="1796" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1796" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1796" t="s">
         <v>1794</v>
       </c>
     </row>
-    <row r="1797" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1797" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1797" t="s">
         <v>1795</v>
       </c>
     </row>
-    <row r="1798" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1798" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1798" t="s">
         <v>1796</v>
       </c>
     </row>
-    <row r="1799" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1799" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1799" t="s">
         <v>1797</v>
       </c>
     </row>
-    <row r="1800" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1800" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1800" t="s">
         <v>1798</v>
       </c>
     </row>
-    <row r="1801" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1801" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1801" t="s">
         <v>1799</v>
       </c>
     </row>
-    <row r="1802" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1802" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1802" t="s">
         <v>1800</v>
       </c>
     </row>
-    <row r="1803" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1803" t="s">
         <v>1801</v>
       </c>
-      <c r="B1803">
+      <c r="C1803">
         <v>659.81</v>
       </c>
-      <c r="C1803">
+      <c r="D1803">
         <v>662.077</v>
       </c>
-      <c r="D1803">
+      <c r="E1803">
         <v>456.01100000000002</v>
       </c>
-      <c r="E1803">
+      <c r="F1803">
         <v>338.66300000000001</v>
       </c>
-    </row>
-    <row r="1804" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1803">
+        <v>325.96100000000001</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1804" t="s">
         <v>1802</v>
       </c>
-      <c r="B1804">
+      <c r="C1804">
         <v>369.29199999999997</v>
       </c>
-      <c r="C1804">
+      <c r="D1804">
         <v>368.40300000000002</v>
       </c>
-      <c r="D1804">
+      <c r="E1804">
         <v>591.76599999999996</v>
       </c>
-      <c r="E1804">
+      <c r="F1804">
         <v>2.7372000000000001</v>
       </c>
-    </row>
-    <row r="1805" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1804">
+        <v>2.6590600000000002</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1805" t="s">
         <v>1803</v>
       </c>
       <c r="B1805">
+        <v>59</v>
+      </c>
+      <c r="C1805">
         <v>0.277785</v>
       </c>
-      <c r="C1805">
+      <c r="D1805">
         <v>0.27700000000000002</v>
       </c>
-      <c r="D1805">
+      <c r="E1805">
         <v>0.434</v>
       </c>
-      <c r="E1805">
+      <c r="F1805">
         <v>8.6759000000000003E-2</v>
       </c>
-    </row>
-    <row r="1806" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1805">
+        <v>8.7472999999999995E-2</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1806" t="s">
         <v>1804</v>
       </c>
       <c r="B1806">
+        <v>56</v>
+      </c>
+      <c r="C1806">
         <v>15.747</v>
       </c>
-      <c r="C1806">
+      <c r="D1806">
         <v>15.744</v>
       </c>
-      <c r="D1806">
+      <c r="E1806">
         <v>15.706300000000001</v>
       </c>
-      <c r="E1806">
+      <c r="F1806">
         <v>8.6440400000000004</v>
       </c>
-    </row>
-    <row r="1807" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1806">
+        <v>8.3489100000000001</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1807" t="s">
         <v>1805</v>
       </c>
       <c r="B1807">
+        <v>60</v>
+      </c>
+      <c r="C1807">
         <v>65.029700000000005</v>
       </c>
-      <c r="C1807">
+      <c r="D1807">
         <v>64.983000000000004</v>
       </c>
-      <c r="D1807">
+      <c r="E1807">
         <v>85.376000000000005</v>
       </c>
-      <c r="E1807">
+      <c r="F1807">
         <v>3.00935</v>
       </c>
-    </row>
-    <row r="1808" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1807">
+        <v>2.9613399999999999</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1808" t="s">
         <v>2002</v>
       </c>
       <c r="B1808">
+        <v>67</v>
+      </c>
+      <c r="C1808">
         <v>0.44271199999999999</v>
       </c>
-      <c r="C1808">
+      <c r="D1808">
         <v>0.44</v>
       </c>
-      <c r="D1808">
+      <c r="E1808">
         <v>0.65100000000000002</v>
       </c>
-      <c r="E1808">
+      <c r="F1808">
         <v>0.114563</v>
       </c>
-    </row>
-    <row r="1809" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1808">
+        <v>0.11154799999999999</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1809" t="s">
         <v>1806</v>
       </c>
-      <c r="C1809">
+      <c r="B1809">
+        <v>44</v>
+      </c>
+      <c r="D1809">
         <v>9.4120000000000002E-3</v>
       </c>
-      <c r="E1809">
+      <c r="F1809">
         <v>2.5256000000000001E-2</v>
       </c>
     </row>
-    <row r="1810" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1810" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1810" t="s">
         <v>1807</v>
       </c>
     </row>
-    <row r="1811" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1811" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1811" t="s">
         <v>1808</v>
       </c>
     </row>
-    <row r="1812" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1812" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1812" t="s">
         <v>1809</v>
       </c>
     </row>
-    <row r="1813" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1813" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1813" t="s">
         <v>1810</v>
       </c>
     </row>
-    <row r="1814" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1814" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1814" t="s">
         <v>1811</v>
       </c>
     </row>
-    <row r="1815" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1815" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1815" t="s">
         <v>1812</v>
       </c>
     </row>
-    <row r="1816" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1816" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1816" t="s">
         <v>1813</v>
       </c>
     </row>
-    <row r="1817" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1817" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1817" t="s">
         <v>1814</v>
       </c>
     </row>
-    <row r="1818" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1818" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1818" t="s">
         <v>1815</v>
       </c>
     </row>
-    <row r="1819" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1819" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1819" t="s">
         <v>1816</v>
       </c>
     </row>
-    <row r="1820" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1820" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1820" t="s">
         <v>1817</v>
       </c>
     </row>
-    <row r="1821" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1821" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1821" t="s">
         <v>1818</v>
       </c>
     </row>
-    <row r="1822" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1822" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1822" t="s">
         <v>1819</v>
       </c>
     </row>
-    <row r="1823" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1823" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1823" t="s">
         <v>1820</v>
       </c>
     </row>
-    <row r="1824" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1824" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1824" t="s">
         <v>1821</v>
       </c>
@@ -19018,198 +19078,198 @@
         <v>1885</v>
       </c>
     </row>
-    <row r="1889" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1889" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1889" t="s">
         <v>1886</v>
       </c>
     </row>
-    <row r="1890" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1890" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1890" t="s">
         <v>1887</v>
       </c>
     </row>
-    <row r="1891" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1891" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1891" t="s">
         <v>1888</v>
       </c>
     </row>
-    <row r="1892" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1892" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1892" t="s">
         <v>1889</v>
       </c>
     </row>
-    <row r="1893" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1893" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1893" t="s">
         <v>1890</v>
       </c>
     </row>
-    <row r="1894" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1894" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1894" t="s">
         <v>1891</v>
       </c>
     </row>
-    <row r="1895" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1895" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1895" t="s">
         <v>1892</v>
       </c>
     </row>
-    <row r="1896" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1896" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1896" t="s">
         <v>1893</v>
       </c>
     </row>
-    <row r="1897" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1897" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1897" t="s">
         <v>1894</v>
       </c>
     </row>
-    <row r="1898" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1898" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1898" t="s">
         <v>1895</v>
       </c>
     </row>
-    <row r="1899" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1899" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1899" t="s">
         <v>1896</v>
       </c>
     </row>
-    <row r="1900" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1900" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1900" t="s">
         <v>1897</v>
       </c>
     </row>
-    <row r="1901" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1901" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1901" t="s">
         <v>1898</v>
       </c>
     </row>
-    <row r="1902" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1902" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1902" t="s">
         <v>1899</v>
       </c>
     </row>
-    <row r="1903" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1903" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1903" t="s">
         <v>1900</v>
       </c>
     </row>
-    <row r="1904" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1904" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1904" t="s">
         <v>1901</v>
       </c>
-      <c r="C1904">
+      <c r="D1904">
         <v>1.1919999999999999</v>
       </c>
-      <c r="E1904">
+      <c r="F1904">
         <v>1.64977</v>
       </c>
     </row>
-    <row r="1905" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1905" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1905" t="s">
         <v>1902</v>
       </c>
-      <c r="C1905">
+      <c r="D1905">
         <v>18.297000000000001</v>
       </c>
-      <c r="E1905">
+      <c r="F1905">
         <v>1023.81</v>
       </c>
     </row>
-    <row r="1906" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1906" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1906" t="s">
         <v>1903</v>
       </c>
-      <c r="C1906">
+      <c r="D1906">
         <v>0.11600000000000001</v>
       </c>
-      <c r="E1906">
+      <c r="F1906">
         <v>3.3174000000000002E-2</v>
       </c>
     </row>
-    <row r="1907" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1907" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1907" t="s">
         <v>1904</v>
       </c>
-      <c r="C1907">
+      <c r="D1907">
         <v>0.39900000000000002</v>
       </c>
-      <c r="E1907">
+      <c r="F1907">
         <v>0.22248699999999999</v>
       </c>
     </row>
-    <row r="1908" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1908" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1908" t="s">
         <v>1905</v>
       </c>
-      <c r="C1908" t="s">
+      <c r="D1908" t="s">
         <v>3007</v>
       </c>
-      <c r="E1908">
+      <c r="F1908">
         <v>0.28599000000000002</v>
       </c>
     </row>
-    <row r="1909" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1909" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1909" t="s">
         <v>1906</v>
       </c>
-      <c r="C1909">
+      <c r="D1909">
         <v>57.531999999999996</v>
       </c>
-      <c r="E1909">
+      <c r="F1909">
         <v>39.853900000000003</v>
       </c>
     </row>
-    <row r="1910" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1910" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1910" t="s">
         <v>1907</v>
       </c>
     </row>
-    <row r="1911" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1911" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1911" t="s">
         <v>1908</v>
       </c>
     </row>
-    <row r="1912" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1912" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1912" t="s">
         <v>1909</v>
       </c>
     </row>
-    <row r="1913" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1913" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1913" t="s">
         <v>1910</v>
       </c>
     </row>
-    <row r="1914" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1914" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1914" t="s">
         <v>1911</v>
       </c>
     </row>
-    <row r="1915" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1915" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1915" t="s">
         <v>1912</v>
       </c>
     </row>
-    <row r="1916" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1916" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1916" t="s">
         <v>1913</v>
       </c>
     </row>
-    <row r="1917" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1917" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1917" t="s">
         <v>1914</v>
       </c>
     </row>
-    <row r="1918" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1918" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1918" t="s">
         <v>1915</v>
       </c>
     </row>
-    <row r="1919" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1919" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1919" t="s">
         <v>1916</v>
       </c>
     </row>
-    <row r="1920" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1920" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1920" t="s">
         <v>1917</v>
       </c>

</xml_diff>

<commit_message>
170	Rename y to input_y.
</commit_message>
<xml_diff>
--- a/benchmark/runtime.xlsx
+++ b/benchmark/runtime.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitcloud\libMultiRobotPlanning\benchmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F7D67E-332C-4A31-9BA2-BA1F97BBA8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF9DA29-CD02-4AB9-8778-52F9DF3B8978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3013" uniqueCount="3010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3014" uniqueCount="3011">
   <si>
     <t>map_8by8_obst12_agents10_ex0.yaml</t>
   </si>
@@ -9060,6 +9060,10 @@
   </si>
   <si>
     <t>cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gloriyo-mine-agent-constraint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -9480,10 +9484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2002"/>
+  <dimension ref="A1:H2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1791" workbookViewId="0">
-      <selection activeCell="B1804" sqref="B1804"/>
+    <sheetView tabSelected="1" topLeftCell="A1789" workbookViewId="0">
+      <selection activeCell="H1809" sqref="H1809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9497,7 +9501,7 @@
     <col min="7" max="7" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2000</v>
       </c>
@@ -9519,78 +9523,81 @@
       <c r="G1" t="s">
         <v>3008</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>3010</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -18487,57 +18494,57 @@
         <v>1790</v>
       </c>
     </row>
-    <row r="1793" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1793" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1793" t="s">
         <v>1791</v>
       </c>
     </row>
-    <row r="1794" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1794" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1794" t="s">
         <v>1792</v>
       </c>
     </row>
-    <row r="1795" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1795" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1795" t="s">
         <v>1793</v>
       </c>
     </row>
-    <row r="1796" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1796" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1796" t="s">
         <v>1794</v>
       </c>
     </row>
-    <row r="1797" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1797" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1797" t="s">
         <v>1795</v>
       </c>
     </row>
-    <row r="1798" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1798" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1798" t="s">
         <v>1796</v>
       </c>
     </row>
-    <row r="1799" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1799" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1799" t="s">
         <v>1797</v>
       </c>
     </row>
-    <row r="1800" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1800" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1800" t="s">
         <v>1798</v>
       </c>
     </row>
-    <row r="1801" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1801" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1801" t="s">
         <v>1799</v>
       </c>
     </row>
-    <row r="1802" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1802" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1802" t="s">
         <v>1800</v>
       </c>
     </row>
-    <row r="1803" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1803" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1803" t="s">
         <v>1801</v>
       </c>
@@ -18556,8 +18563,11 @@
       <c r="G1803">
         <v>325.96100000000001</v>
       </c>
-    </row>
-    <row r="1804" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1803">
+        <v>317.03899999999999</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1804" t="s">
         <v>1802</v>
       </c>
@@ -18576,8 +18586,11 @@
       <c r="G1804">
         <v>2.6590600000000002</v>
       </c>
-    </row>
-    <row r="1805" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1804">
+        <v>2.6042800000000002</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1805" t="s">
         <v>1803</v>
       </c>
@@ -18599,8 +18612,11 @@
       <c r="G1805">
         <v>8.7472999999999995E-2</v>
       </c>
-    </row>
-    <row r="1806" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1805">
+        <v>8.2693000000000003E-2</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1806" t="s">
         <v>1804</v>
       </c>
@@ -18622,8 +18638,11 @@
       <c r="G1806">
         <v>8.3489100000000001</v>
       </c>
-    </row>
-    <row r="1807" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1806">
+        <v>8.2100000000000009</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1807" t="s">
         <v>1805</v>
       </c>
@@ -18645,8 +18664,11 @@
       <c r="G1807">
         <v>2.9613399999999999</v>
       </c>
-    </row>
-    <row r="1808" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1807">
+        <v>2.9404699999999999</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1808" t="s">
         <v>2002</v>
       </c>
@@ -18667,6 +18689,9 @@
       </c>
       <c r="G1808">
         <v>0.11154799999999999</v>
+      </c>
+      <c r="H1808">
+        <v>0.10934000000000001</v>
       </c>
     </row>
     <row r="1809" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>